<commit_message>
-updated with final project grade w/ comments
</commit_message>
<xml_diff>
--- a/Journal/Feedback.xlsx
+++ b/Journal/Feedback.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6444EF-D270-4F63-8FC1-2D07EE73BF50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,17 +13,23 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>Team</t>
   </si>
@@ -136,12 +143,27 @@
   </si>
   <si>
     <t>Nathan</t>
+  </si>
+  <si>
+    <t>separate branches remained with entire result</t>
+  </si>
+  <si>
+    <t>not done</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>no code commited, but some research done on collision detection</t>
+  </si>
+  <si>
+    <t>no code commited, but some research done bill boarding for particles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$-409]dddd\,\ m/dd"/>
@@ -573,7 +595,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -633,6 +661,138 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2828925</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3467100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D81325F-6DC5-4707-A349-DE0F856944E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8420100" y="3771900"/>
+          <a:ext cx="2828925" cy="3467100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>-FR1 some class based code, most drawing still done in using direct</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> OGL calles in main routine</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>-FR2 some class abstraction, most camera manipulation done using direct OGL calls in main routine</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>-FR3 complete .   Used third-party file parser, converted between data structures</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>-FR4 very partial attempt at implementing s.g. structure</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>-FR5 no s.g. loading, just per model loading</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>-FR6 not attempted</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>-FR7 no class abstraction, lighting still mostly direct OGL calls</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>-FR9 attempt and partial success in separate git branch</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>-FR10 not attempted</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -640,74 +800,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Schedule"/>
-      <sheetName val="Students"/>
-      <sheetName val="Canvas - Import"/>
-      <sheetName val="Deliverables"/>
-      <sheetName val="Projects"/>
       <sheetName val="Px Lighting"/>
-      <sheetName val="Px Lighting - Schedule"/>
-      <sheetName val="Px Lighting - Parts"/>
-      <sheetName val="Project Grade What If"/>
-      <sheetName val="Sheet4"/>
-      <sheetName val="Mid-Semester Results"/>
-      <sheetName val="Mid-Semester Results - Import"/>
-      <sheetName val="Partial-Semester Results"/>
-      <sheetName val="Partial Semester - Import"/>
-      <sheetName val="Semester Results"/>
-      <sheetName val="Semester Results - Import"/>
-      <sheetName val="End-Semester Results"/>
-      <sheetName val="End-Semester Results - Import"/>
-      <sheetName val="Midterm"/>
-      <sheetName val="3-4 Term"/>
-      <sheetName val="Final"/>
-      <sheetName val="Mid Semester"/>
-      <sheetName val="Student Email"/>
-      <sheetName val="Scrap"/>
-      <sheetName val="Student List - Import"/>
-      <sheetName val="Student Email - Import"/>
-      <sheetName val="Results.old"/>
-      <sheetName val="Project 1.old"/>
-      <sheetName val="Git Export"/>
-      <sheetName val="Git Repos"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet3"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -975,11 +1071,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,7 +1083,7 @@
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="23.5703125" customWidth="1"/>
     <col min="10" max="10" width="7.5703125" customWidth="1"/>
     <col min="11" max="11" width="43.42578125" customWidth="1"/>
@@ -1135,7 +1231,9 @@
       <c r="I7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="18"/>
+      <c r="J7" s="18">
+        <v>10</v>
+      </c>
       <c r="K7" s="19" t="s">
         <v>14</v>
       </c>
@@ -1173,7 +1271,7 @@
       </c>
       <c r="K8" s="29"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="281.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30">
         <v>3</v>
       </c>
@@ -1201,10 +1299,13 @@
       <c r="I9" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="38"/>
+      <c r="J9" s="38">
+        <f>D9*0.75</f>
+        <v>18.75</v>
+      </c>
       <c r="K9" s="39"/>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="30">
         <v>4</v>
       </c>
@@ -1232,10 +1333,14 @@
       <c r="I10" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="40"/>
-      <c r="K10" s="41"/>
+      <c r="J10" s="40">
+        <v>2</v>
+      </c>
+      <c r="K10" s="41" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="30">
         <v>5</v>
       </c>
@@ -1263,10 +1368,15 @@
       <c r="I11" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="37"/>
-      <c r="K11" s="41"/>
+      <c r="J11" s="37">
+        <f>23*0.25</f>
+        <v>5.75</v>
+      </c>
+      <c r="K11" s="41" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="30">
         <v>6</v>
       </c>
@@ -1294,10 +1404,14 @@
       <c r="I12" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="40"/>
-      <c r="K12" s="41"/>
+      <c r="J12" s="40">
+        <v>0</v>
+      </c>
+      <c r="K12" s="41" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="30">
         <v>7</v>
       </c>
@@ -1325,8 +1439,13 @@
       <c r="I13" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="37"/>
-      <c r="K13" s="41"/>
+      <c r="J13" s="37">
+        <f>23*0.25</f>
+        <v>5.75</v>
+      </c>
+      <c r="K13" s="41" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
@@ -1356,8 +1475,12 @@
       <c r="I14" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="37"/>
-      <c r="K14" s="41"/>
+      <c r="J14" s="37">
+        <v>2.5</v>
+      </c>
+      <c r="K14" s="41" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="30">
@@ -1387,7 +1510,9 @@
       <c r="I15" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="J15" s="42"/>
+      <c r="J15" s="42">
+        <v>5</v>
+      </c>
       <c r="K15" s="41"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1417,7 +1542,7 @@
       </c>
       <c r="J17" s="3">
         <f>SUM(J8:J15)</f>
-        <v>5</v>
+        <v>44.75</v>
       </c>
       <c r="K17" s="2"/>
     </row>
@@ -1440,7 +1565,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="2" operator="containsText" text="0" id="{B0E73979-B11A-4233-91AE-797BB8BA3FED}">
-            <xm:f>NOT(ISERROR(SEARCH("0",'\Users\zwartell\Dropbox (UNC Charlotte)\classes\ITCS_x120.git\planning\[3120 Fall 2018 - Planner.xlsx]Px Lighting'!#REF!)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH("0",'C:\Users\zwartell\Dropbox (UNC Charlotte)\classes\ITCS_x120.git\planning\[3120 Fall 2018 - Planner.xlsx]Px Lighting'!#REF!)))</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -1456,7 +1581,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="4" operator="containsText" text="0" id="{DFECA1A2-139A-4031-BE70-175699D69D21}">
-            <xm:f>NOT(ISERROR(SEARCH("0",'\Users\zwartell\Dropbox (UNC Charlotte)\classes\ITCS_x120.git\planning\[3120 Fall 2018 - Planner.xlsx]Px Lighting'!#REF!)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH("0",'C:\Users\zwartell\Dropbox (UNC Charlotte)\classes\ITCS_x120.git\planning\[3120 Fall 2018 - Planner.xlsx]Px Lighting'!#REF!)))</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>

</xml_diff>